<commit_message>
lab6 report & little updates
</commit_message>
<xml_diff>
--- a/Lab6/Experiment Results/Lab6 Results.xlsx
+++ b/Lab6/Experiment Results/Lab6 Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FAACFA-A850-4365-B441-F520E2DBF694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34462204-96B0-4171-B411-565D7B523328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Exp No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Epsilon </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Adam</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +91,10 @@
   </si>
   <si>
     <t>nan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Episode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -466,16 +466,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -496,10 +496,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -518,8 +518,11 @@
       <c r="E2" s="2">
         <v>128</v>
       </c>
+      <c r="F2" s="2">
+        <v>10000</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>0.995</v>
@@ -548,13 +551,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>2000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>64</v>
@@ -563,13 +566,13 @@
         <v>500000</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="2">
         <v>0.99</v>
@@ -585,6 +588,47 @@
       </c>
       <c r="N3" s="2">
         <v>263.41599992959601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>128</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.995</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exp5 result & lab6 report update
</commit_message>
<xml_diff>
--- a/Lab6/Experiment Results/Lab6 Results.xlsx
+++ b/Lab6/Experiment Results/Lab6 Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8403853-B142-4B05-B340-49246E4DD089}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD00F0-EB7C-4E6D-85FF-9743F66B5F68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Exp No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -724,6 +724,56 @@
       <c r="M6" s="2">
         <v>1E-3</v>
       </c>
+      <c r="N6" s="2">
+        <v>266.82029999999997</v>
+      </c>
+      <c r="O6" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2">
+        <v>500000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="O7" s="2">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>